<commit_message>
refactor: PersonnelForm sub-components + React Query integration
</commit_message>
<xml_diff>
--- a/employeeImportTemplate.xlsx
+++ b/employeeImportTemplate.xlsx
@@ -1,41 +1,145 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QuocAnh\cic-erp-contract\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="16980"/>
+  </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t>Mã NV *</t>
+  </si>
+  <si>
+    <t>Họ và tên *</t>
+  </si>
+  <si>
+    <t>Email *</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Telegram</t>
+  </si>
+  <si>
+    <t>Chức vụ</t>
+  </si>
+  <si>
+    <t>Role *</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Số CCCD</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Trình độ học vấn</t>
+  </si>
+  <si>
+    <t>Chuyên ngành</t>
+  </si>
+  <si>
+    <t>Chứng chỉ</t>
+  </si>
+  <si>
+    <t>Ngày vào làm</t>
+  </si>
+  <si>
+    <t>Loại hợp đồng</t>
+  </si>
+  <si>
+    <t>Số tài khoản NH</t>
+  </si>
+  <si>
+    <t>Tên ngân hàng</t>
+  </si>
+  <si>
+    <t>NV001</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>a@cic.vn</t>
+  </si>
+  <si>
+    <t>0901234567</t>
+  </si>
+  <si>
+    <t>@nguyen_a</t>
+  </si>
+  <si>
+    <t>bim</t>
+  </si>
+  <si>
+    <t>Chuyên viên</t>
+  </si>
+  <si>
+    <t>NVKD</t>
+  </si>
+  <si>
+    <t>15/03/1990</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>001234567890</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>Đại học</t>
+  </si>
+  <si>
+    <t>CNTT</t>
+  </si>
+  <si>
+    <t>PMP</t>
+  </si>
+  <si>
+    <t>01/01/2024</t>
+  </si>
+  <si>
+    <t>Full-time</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>VCB</t>
+  </si>
+  <si>
+    <t>Tên đơn vị</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +176,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,115 +508,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1048576"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="7" width="15.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Mã nhân viên *</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Họ và tên *</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Email *</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Số điện thoại</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Mã đơn vị *</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Chức vụ</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Role *</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Ngày sinh</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Giới tính</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Số CCCD</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Địa chỉ</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Trình độ học vấn</v>
-      </c>
-      <c r="M1" t="str">
-        <v>Ngày vào làm</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Loại hợp đồng</v>
-      </c>
-      <c r="O1" t="str">
-        <v>Số tài khoản NH</v>
-      </c>
-      <c r="P1" t="str">
-        <v>Tên ngân hàng</v>
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>NV001</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Nguyễn Văn A</v>
-      </c>
-      <c r="C2" t="str">
-        <v>a@cic.vn</v>
-      </c>
-      <c r="D2" t="str">
-        <v>0901234567</v>
-      </c>
-      <c r="E2" t="str">
-        <v>bim</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Chuyên viên</v>
-      </c>
-      <c r="G2" t="str">
-        <v>NVKD</v>
-      </c>
-      <c r="H2" t="str">
-        <v>15/03/1990</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Nam</v>
-      </c>
-      <c r="J2" t="str">
-        <v>001234567890</v>
-      </c>
-      <c r="K2" t="str">
-        <v>Hà Nội</v>
-      </c>
-      <c r="L2" t="str">
-        <v>Đại học</v>
-      </c>
-      <c r="M2" t="str">
-        <v>01/01/2024</v>
-      </c>
-      <c r="N2" t="str">
-        <v>Chính thức</v>
-      </c>
-      <c r="O2" t="str">
-        <v>1234567890</v>
-      </c>
-      <c r="P2" t="str">
-        <v>VCB</v>
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
+    <ignoredError sqref="A1:E1 A2:E2 G2:S2 G1:S1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>